<commit_message>
Updated the exception handling
</commit_message>
<xml_diff>
--- a/SVCareers_Automation_Testing_Project/Data/CreateJobRequest.xlsx
+++ b/SVCareers_Automation_Testing_Project/Data/CreateJobRequest.xlsx
@@ -212,7 +212,7 @@
     <t>Addtional Billing</t>
   </si>
   <si>
-    <t>SFGTest4</t>
+    <t>SFGTest11</t>
   </si>
 </sst>
 </file>
@@ -571,7 +571,7 @@
   <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>